<commit_message>
Se realizan mejoras modulo Analisis de Riesgos
</commit_message>
<xml_diff>
--- a/storage/app/public/exportExcel/analisis_riesgo.xlsx
+++ b/storage/app/public/exportExcel/analisis_riesgo.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\tabantaj\storage\app\public\exportExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\tabantaj\public\storage\exportExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3498BC-6366-406C-B271-7727C7DC9DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="855" yWindow="1560" windowWidth="20040" windowHeight="8595"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,37 +20,45 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Seguridad de la información</t>
-  </si>
-  <si>
-    <t>Vigente</t>
-  </si>
-  <si>
-    <t>Prueba Pedro</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Nombre (texto)</t>
+  </si>
+  <si>
+    <t>Porcentaje Implementacion (numero)</t>
+  </si>
+  <si>
+    <t>ID Empleado que elaboro (numero)</t>
+  </si>
+  <si>
+    <t>Estatus (Texto)</t>
+  </si>
+  <si>
+    <t>Fecha (AAAA-MM-DD)</t>
+  </si>
+  <si>
+    <t>ID Tipo (Numero</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -66,7 +75,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -83,9 +92,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
@@ -401,50 +411,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7265625" customWidth="1"/>
+    <col min="4" max="4" width="33.36328125" customWidth="1"/>
+    <col min="5" max="5" width="31.1796875" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3">
-        <v>44477</v>
-      </c>
-      <c r="D1" s="2">
-        <v>30</v>
-      </c>
-      <c r="E1" s="2">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>1</v>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C2" s="1"/>
+      <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>